<commit_message>
Troca google pela hostinger
</commit_message>
<xml_diff>
--- a/backend/rdd/RDD-Brejinho.xlsx
+++ b/backend/rdd/RDD-Brejinho.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>TIPO_DE_SERVICO</t>
   </si>
@@ -34,82 +34,22 @@
     <t>DATA</t>
   </si>
   <si>
-    <t>Manutenção no equipamento da cliente</t>
-  </si>
-  <si>
-    <t>Vila de fatima</t>
-  </si>
-  <si>
-    <t>10:56</t>
-  </si>
-  <si>
-    <t>13:47</t>
-  </si>
-  <si>
-    <t>02:51</t>
-  </si>
-  <si>
-    <t>Rivaldo Souza</t>
-  </si>
-  <si>
-    <t>22/4/2022</t>
-  </si>
-  <si>
-    <t>Manutenção na antena e no Ap da cliente</t>
-  </si>
-  <si>
-    <t>Lagoa dos campos</t>
-  </si>
-  <si>
-    <t>10:31</t>
-  </si>
-  <si>
-    <t>14:57</t>
-  </si>
-  <si>
-    <t>04:26</t>
-  </si>
-  <si>
-    <t>Explicação a respeito do tvbox</t>
-  </si>
-  <si>
-    <t>Brejinho</t>
-  </si>
-  <si>
-    <t>09:50</t>
-  </si>
-  <si>
-    <t>11:56</t>
-  </si>
-  <si>
-    <t>02:06</t>
-  </si>
-  <si>
-    <t>Atendimento preliminar transferencia para o financeiro</t>
-  </si>
-  <si>
-    <t>14:16</t>
-  </si>
-  <si>
-    <t>14:44</t>
-  </si>
-  <si>
-    <t>00:28</t>
-  </si>
-  <si>
-    <t>Manotenção no roteador do cliente</t>
-  </si>
-  <si>
-    <t>Vila de Fatima</t>
-  </si>
-  <si>
-    <t>08:43</t>
-  </si>
-  <si>
-    <t>09:09</t>
-  </si>
-  <si>
-    <t>00:26</t>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>01:00</t>
+  </si>
+  <si>
+    <t>Rivaldo</t>
+  </si>
+  <si>
+    <t>26/4/2022</t>
   </si>
 </sst>
 </file>
@@ -496,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="60" customWidth="1"/>
@@ -531,114 +471,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>